<commit_message>
upto State and Lifecycle
</commit_message>
<xml_diff>
--- a/ReactMindMap.xlsx
+++ b/ReactMindMap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t>Stateful component</t>
   </si>
@@ -173,7 +173,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Rendering</t>
+      <t>React</t>
     </r>
     <r>
       <rPr>
@@ -198,17 +198,207 @@
     </r>
   </si>
   <si>
-    <t>describes what you want to see on screen</t>
-  </si>
-  <si>
-    <t>smallest building block, plain object, cheap to create</t>
+    <t>ReactDOM.render(
+  element,
+  document.getElementById('root')
+);</t>
+  </si>
+  <si>
+    <t>React elements are immutable.</t>
+  </si>
+  <si>
+    <t>The only way to update the UI is to create a new element, and pass it to ReactDOM.render().</t>
+  </si>
+  <si>
+    <t>React Only Updates What’s Necessary</t>
+  </si>
+  <si>
+    <t>Describes what you want to see on screen</t>
+  </si>
+  <si>
+    <r>
+      <t>In practice, most React apps only call</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ReactDOM.render()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> once.  ==&gt;&gt; code gets encapsulated into stateful components.</t>
+    </r>
+  </si>
+  <si>
+    <t>Smallest building block, plain object, cheap to create</t>
+  </si>
+  <si>
+    <t>React DOM takes care of updating the DOM to match the React elements.</t>
+  </si>
+  <si>
+    <t>Components and Props</t>
+  </si>
+  <si>
+    <t>Components let you split the UI into independent, reusable pieces, and think about each piece in isolation.</t>
+  </si>
+  <si>
+    <t>class Welcome extends React.Component {
+  render() {
+    return &lt;h1&gt;Hello, {this.props.name}&lt;/h1&gt;;
+  }
+}</t>
+  </si>
+  <si>
+    <t>Function component</t>
+  </si>
+  <si>
+    <t>can render DOM tags + user defined components</t>
+  </si>
+  <si>
+    <t>function Welcome(props) {
+  return &lt;h1&gt;Hello, {props.name}&lt;/h1&gt;;
+}
+const element = &lt;Welcome name="Sara" /&gt;;
+ReactDOM.render(
+  element,
+  document.getElementById('root')
+);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Conceptually, components are like JavaScript functions, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I/P(Props)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>O/P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(React elements describing what should appear on the screen.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.  We call ReactDOM.render() with the &lt;Welcome name="Sara" /&gt; element.
+2.  React calls the Welcome component with {name: 'Sara'} as the props.
+3.  Our Welcome component returns a &lt;h1&gt;Hello, Sara&lt;/h1&gt; element as the result.
+4.  React DOM efficiently updates the DOM to match &lt;h1&gt;Hello, Sara&lt;/h1&gt;.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Always start component names with a capital letter.</t>
+    </r>
+  </si>
+  <si>
+    <t>Components can refer to other components in their output.</t>
+  </si>
+  <si>
+    <t>Props naming ==&gt;&gt; component’s own point of view rather than the context in which it is being used.</t>
+  </si>
+  <si>
+    <t>Props are Read-Only</t>
+  </si>
+  <si>
+    <t>State and Lifecycle</t>
+  </si>
+  <si>
+    <t>State is similar to props, but it is private and fully controlled by the component.</t>
+  </si>
+  <si>
+    <t>Do Not Modify State Directly</t>
+  </si>
+  <si>
+    <t>// Wrong
+this.state.comment = 'Hello';
+// Correct
+this.setState({comment: 'Hello'});</t>
+  </si>
+  <si>
+    <t>The only place where you can assign this.state is the constructor.</t>
+  </si>
+  <si>
+    <t>State Updates are Merged</t>
+  </si>
+  <si>
+    <t>The merging is shallow, so this.setState({comments}) leaves this.state.posts intact, but completely replaces this.state.comments.</t>
+  </si>
+  <si>
+    <t>A component may choose to pass its state down as props to its child components:</t>
+  </si>
+  <si>
+    <t>You can use stateless components inside stateful components, and vice versa.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +427,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -264,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -286,6 +481,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,15 +962,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="100.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59.28515625" customWidth="1"/>
   </cols>
@@ -834,22 +1041,152 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>54</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>48</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C17" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="C25" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="12"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="12"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="12"/>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="12"/>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D2:D5"/>
+    <mergeCell ref="D30:D35"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:D1">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
upto 9 list and keys
</commit_message>
<xml_diff>
--- a/ReactMindMap.xlsx
+++ b/ReactMindMap.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="8205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Random" sheetId="1" r:id="rId1"/>
-    <sheet name="React-MainConcepts" sheetId="2" r:id="rId2"/>
+    <sheet name="React-16.5.2-MainConcepts" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="ReactDocs">'React-16.5.2-MainConcepts'!$1:$1048576</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="99">
   <si>
     <t>Stateful component</t>
   </si>
@@ -393,12 +396,117 @@
   <si>
     <t>You can use stateless components inside stateful components, and vice versa.</t>
   </si>
+  <si>
+    <t>Handling Events</t>
+  </si>
+  <si>
+    <t>React events are named using camelCase, rather than lowercase.</t>
+  </si>
+  <si>
+    <t>With JSX you pass a function as the event handler, rather than a string.</t>
+  </si>
+  <si>
+    <t>&lt;button onClick={activateLasers}&gt; Activate Lasers&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cannot return false to prevent default behavior in React. You must call preventDefault explicitly.</t>
+  </si>
+  <si>
+    <t>event obj passed to handler is synthetic event</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Conditional</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rendering</t>
+    </r>
+  </si>
+  <si>
+    <t>Preventing Component from Rendering. Return null from render() method of component</t>
+  </si>
+  <si>
+    <t>can render component in if/else or for loop</t>
+  </si>
+  <si>
+    <t>Returning null from a component’s render method does not affect the firing of the component’s lifecycle methods. For instance componentDidUpdate will still be called.</t>
+  </si>
+  <si>
+    <t>Lists and Keys</t>
+  </si>
+  <si>
+    <t>Keys</t>
+  </si>
+  <si>
+    <t>Keys help React identify which items have changed, are added, or are removed</t>
+  </si>
+  <si>
+    <t>Keys give the array elements a stable identity</t>
+  </si>
+  <si>
+    <t>not recommend using indexes for keys if the order of items may change.</t>
+  </si>
+  <si>
+    <t>https://medium.com/@robinpokorny/index-as-a-key-is-an-anti-pattern-e0349aece318</t>
+  </si>
+  <si>
+    <t>https://reactjs.org/docs/reconciliation.html#recursing-on-children</t>
+  </si>
+  <si>
+    <t>A good rule of thumb is that elements inside the map() call need keys.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">identifies a list item among its siblings. </t>
+  </si>
+  <si>
+    <t>We can use the same keys when we produce two different arrays</t>
+  </si>
+  <si>
+    <t>Keys serve as a hint to React but they don’t get passed to your components. If you need the same value in your component, pass it explicitly as a prop with a different name</t>
+  </si>
+  <si>
+    <t>const content = posts.map((post) =&gt;
+  &lt;Post
+    key={post.id}
+    id={post.id}
+    title={post.title} /&gt;
+);</t>
+  </si>
+  <si>
+    <t>Keep in mind that if the map() body is too nested, it might be a good time to extract a component.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +540,14 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -456,10 +572,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -476,9 +593,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -493,8 +607,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -502,6 +627,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -550,7 +678,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -585,7 +713,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -962,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B56" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,25 +1104,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="12" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1002,19 +1130,19 @@
       <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="12"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -1048,7 +1176,7 @@
       <c r="C12" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1073,7 +1201,7 @@
       </c>
     </row>
     <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1083,7 +1211,7 @@
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C20" t="s">
@@ -1099,13 +1227,13 @@
       <c r="C22" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1115,10 +1243,10 @@
       </c>
     </row>
     <row r="25" spans="2:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="9" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1138,13 +1266,13 @@
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C30" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="13" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1152,41 +1280,142 @@
       <c r="C31" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="12"/>
+      <c r="D31" s="13"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="12"/>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="12"/>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="12"/>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="12"/>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="13"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>75</v>
       </c>
     </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="14"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C44" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C53" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="D30:D35"/>
+    <mergeCell ref="D38:D39"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:D1">
     <cfRule type="colorScale" priority="1">
@@ -1200,8 +1429,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D50" r:id="rId1"/>
+    <hyperlink ref="D46" r:id="rId2" location="recursing-on-children"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
upto composition vs inheritance.
</commit_message>
<xml_diff>
--- a/ReactMindMap.xlsx
+++ b/ReactMindMap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="8205" activeTab="1"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Random" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
   <si>
     <t>Stateful component</t>
   </si>
@@ -500,6 +500,122 @@
   </si>
   <si>
     <t>Keep in mind that if the map() body is too nested, it might be a good time to extract a component.</t>
+  </si>
+  <si>
+    <t>Composition vs Inheritance</t>
+  </si>
+  <si>
+    <t>Lifting state up</t>
+  </si>
+  <si>
+    <t>React has a powerful composition model, and we recommend using composition instead of inheritance to reuse code between components.</t>
+  </si>
+  <si>
+    <t>function FancyBorder(props) {
+  return (
+    &lt;div className={'FancyBorder FancyBorder-' + props.color}&gt;
+      {props.children}
+    &lt;/div&gt;
+  );
+}</t>
+  </si>
+  <si>
+    <t>Some components don’t know their children ahead of time. This is especially common for components like Sidebar or Dialog that represent generic “boxes”.
+We recommend that such components use the special children prop to pass children elements directly into their output:
+This lets other components pass arbitrary children to them by nesting the JSX</t>
+  </si>
+  <si>
+    <t>In React, this is also achieved by composition, where a more “specific” component renders a more “generic” one and configures it with props:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Containment and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Children</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> property</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Specialization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Sometimes we think about components as being “special cases” of other components</t>
+    </r>
+  </si>
+  <si>
+    <t>Composition works equally well for components defined as classes</t>
+  </si>
+  <si>
+    <t>So What About Inheritance?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Props and composition give you all the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>flexibility</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> you need to customize a component’s look and behavior in an explicit and safe way. Remember that components may accept arbitrary props, including primitive values, React elements, or functions.</t>
+    </r>
+  </si>
+  <si>
+    <t>If you want to reuse non-UI functionality between components, we suggest extracting it into a separate JavaScript module. The components may import it and use that function, object, or a class, without extending it.</t>
+  </si>
+  <si>
+    <t>Thinking in React</t>
+  </si>
+  <si>
+    <t>Start With A Mock</t>
   </si>
 </sst>
 </file>
@@ -576,7 +692,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -608,6 +724,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -616,7 +736,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1090,15 +1209,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B56" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="100.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59.28515625" customWidth="1"/>
   </cols>
@@ -1122,7 +1241,7 @@
       <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="14" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1130,19 +1249,19 @@
       <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="12"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -1272,7 +1391,7 @@
       <c r="C30" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1280,31 +1399,31 @@
       <c r="C31" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="13"/>
+      <c r="D31" s="15"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="13"/>
+      <c r="D32" s="15"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="13"/>
+      <c r="D33" s="15"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="13"/>
+      <c r="D34" s="15"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="13"/>
+      <c r="D35" s="15"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
@@ -1318,7 +1437,7 @@
       <c r="C38" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="16" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1326,7 +1445,7 @@
       <c r="C39" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="14"/>
+      <c r="D39" s="16"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
@@ -1361,7 +1480,7 @@
       <c r="C46" t="s">
         <v>87</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="13" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1375,30 +1494,30 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="3:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="C53" s="11" t="s">
         <v>96</v>
       </c>
@@ -1406,9 +1525,73 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="C60" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="C65" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="C66" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upto Thinking in React
</commit_message>
<xml_diff>
--- a/ReactMindMap.xlsx
+++ b/ReactMindMap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8205" activeTab="1"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Random" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="120">
   <si>
     <t>Stateful component</t>
   </si>
@@ -616,6 +616,29 @@
   </si>
   <si>
     <t>Start With A Mock</t>
+  </si>
+  <si>
+    <t>Step 1: Break The UI Into A Component Hierarchy</t>
+  </si>
+  <si>
+    <t>Step 2: Build A Static Version in React</t>
+  </si>
+  <si>
+    <t>Step 3: Identify The Minimal (but complete) Representation Of UI State</t>
+  </si>
+  <si>
+    <t>1. Is it passed in from a parent via props? If so, it probably isn’t state.
+2. Does it remain unchanged over time? If so, it probably isn’t state
+3. Can you compute it based on any other state or props in your component? If so, it isn’t state.</t>
+  </si>
+  <si>
+    <t>Step 4: Identify Where Your State Should Live</t>
+  </si>
+  <si>
+    <t>Step 5: Add Inverse Data Flow</t>
+  </si>
+  <si>
+    <t>And That’s It</t>
   </si>
 </sst>
 </file>
@@ -692,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -735,6 +758,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1209,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,29 +1603,66 @@
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C65" s="9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="66" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C66" s="9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="7" t="s">
         <v>111</v>
       </c>
       <c r="C68" t="s">
         <v>112</v>
       </c>
+      <c r="D68" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>113</v>
+      </c>
+      <c r="D69" s="17"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>114</v>
+      </c>
+      <c r="D70" s="17"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>115</v>
+      </c>
+      <c r="D71" s="17"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="D30:D35"/>
     <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D68:D71"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:D1">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
updated SASS and JS sections
</commit_message>
<xml_diff>
--- a/ReactMindMap.xlsx
+++ b/ReactMindMap.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="5310" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="5310" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Random" sheetId="1" r:id="rId1"/>
     <sheet name="React-16.5.2-MainConcepts" sheetId="2" r:id="rId2"/>
     <sheet name="Advanced concepts" sheetId="3" r:id="rId3"/>
-    <sheet name="Sass" sheetId="4" r:id="rId4"/>
+    <sheet name="JavaScript" sheetId="6" r:id="rId4"/>
+    <sheet name="Sass" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="8" r:id="rId6"/>
+    <sheet name="HTML" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="ReactDocs">'React-16.5.2-MainConcepts'!$1:$1048576</definedName>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="324">
   <si>
     <t>Stateful component</t>
   </si>
@@ -1794,32 +1797,337 @@
     <t>@extend</t>
   </si>
   <si>
-    <t>meta tag</t>
-  </si>
-  <si>
     <t>box sizing: borderbox</t>
   </si>
   <si>
     <t>col define: 12 column 100%</t>
   </si>
   <si>
-    <t>clear float after row</t>
-  </si>
-  <si>
-    <t>all col add upto and within row</t>
-  </si>
-  <si>
-    <t>images</t>
-  </si>
-  <si>
     <t>max-width:100%</t>
+  </si>
+  <si>
+    <t>all col add upto 12 and within row</t>
+  </si>
+  <si>
+    <t>images, videos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audio video support </t>
+  </si>
+  <si>
+    <t>application cache and SQL DB</t>
+  </si>
+  <si>
+    <t>HTML5</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>supported with flash player</t>
+  </si>
+  <si>
+    <t>cookies</t>
+  </si>
+  <si>
+    <t>support using various api like VML, flash, Silverlight</t>
+  </si>
+  <si>
+    <t>Drag and drop</t>
+  </si>
+  <si>
+    <t>not supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geolocation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not possible to get true location </t>
+  </si>
+  <si>
+    <t>mobile friendly</t>
+  </si>
+  <si>
+    <t>not mobile friendly</t>
+  </si>
+  <si>
+    <t>Vector graphics:  canvas, svg</t>
+  </si>
+  <si>
+    <t>Semantic tags</t>
+  </si>
+  <si>
+    <t>Styled Components</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">styled-components utilises </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tagged template literals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to style your components.
+It removes the mapping between components and styles. This means that when you're defining your styles, you're actually creating a normal React component, that has your styles attached to it.</t>
+    </r>
+  </si>
+  <si>
+    <t>withRouter() from 'react-router-dom';</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Primitive data type
+2. Return a unique symbol value
+3. primary purpose: used as an identifier for object properties
+4. </t>
+  </si>
+  <si>
+    <t>let sym1 = Symbol()
+let sym2 = Symbol('foo')
+let sym3 = Symbol('foo')
+foo is ==&gt;  optional description, but for debugging purposes only.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Generator fn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich content </t>
+  </si>
+  <si>
+    <t>Better symantic</t>
+  </si>
+  <si>
+    <t>Stricter parsing to simlify error handling</t>
+  </si>
+  <si>
+    <t>Bette cross Plateform support</t>
+  </si>
+  <si>
+    <t>Diff bet HTML and HTML5</t>
+  </si>
+  <si>
+    <t>Canvas</t>
+  </si>
+  <si>
+    <t>&lt;canvas id="c" width="300" height="300"&gt;&lt;/canvas&gt;
+&lt;script&gt;
+  var canvas = document.getElementById( "c" );
+  var drawing_context = canvas.getContext( "2d" );
+  drawing_context.fillStyle = "blue";
+  drawing_context.fillRect( 50, 50, 100, 100 );
+&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>LocalStorage</t>
+  </si>
+  <si>
+    <t>documents with different origins will never share the stored objects</t>
+  </si>
+  <si>
+    <t>sessionStorage</t>
+  </si>
+  <si>
+    <t>sessionStorage is also scoped on a per-window basis. If a user has two browser tabs displaying documents from the same origin, those two tabs have separate sessionStorage data: the scripts running in one tab cannot read or overwrite the data written by scripts in the other tab, even if both tabs are visiting exactly the same page and are running exactly the same scripts.</t>
+  </si>
+  <si>
+    <t>If a user has two browser tabs displaying documents from the same origin, those two tabs have shared localStorage data</t>
+  </si>
+  <si>
+    <t>SVG vs Canvas</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The &lt;svg&gt; element is a container for SVG graphics. SVG has several methods for drawing paths, boxes, circles, text, and even bitmap images.
+SVG is a language for describing 2D graphics, 
+SVG is XML-based, which means that every element is available within the SVG DOM. You can attach JavaScript event handlers for an element.
+In SVG, each drawn shape is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>remembered</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as an object. If attributes of an SVG object are changed, the browser can automatically re-render the shape.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;canvas&gt; allows you to draw 2D graphics on the fly using JavaScript.
+Canvas is rendered pixel by pixel. In canvas, once the graphic is drawn, it is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>forgotten</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> by the browser. If its position should be changed, the entire scene needs to be redrawn, including any objects that might have been covered by the graphic.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Resonsive layout</t>
+  </si>
+  <si>
+    <t>float: left</t>
+  </si>
+  <si>
+    <t>Responsive Text</t>
+  </si>
+  <si>
+    <t>vw : viewport width</t>
+  </si>
+  <si>
+    <t>&lt;picture&gt;
+  &lt;source srcset="img_smallflower.jpg" media="(max-width: 600px)"&gt;
+  &lt;source srcset="img_flowers.jpg" media="(max-width: 1500px)"&gt;
+  &lt;source srcset="flowers.jpg"&gt;
+  &lt;img src="img_smallflower.jpg" alt="Flowers"&gt;
+&lt;/picture&gt;</t>
+  </si>
+  <si>
+    <t>meta viewort tag</t>
+  </si>
+  <si>
+    <t>control the page's dimensions and scaling.</t>
+  </si>
+  <si>
+    <t>Size Content to The Viewport</t>
+  </si>
+  <si>
+    <t>1. Do NOT use large fixed width elements
+2. Do NOT let the content rely on a particular viewport width to render well 
+3. Use CSS media queries to apply different styling for small and large screens</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;picture&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>element allows you to define different images for different browser window sizes.</t>
+    </r>
+  </si>
+  <si>
+    <t>clear float in row::after</t>
+  </si>
+  <si>
+    <t>Always Design for Mobile First</t>
+  </si>
+  <si>
+    <t>Add breakpoints: media queries</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>parent selector</t>
+  </si>
+  <si>
+    <r>
+      <t>The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2E2F3E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&amp; always refers to the parent selector when nesting. Think of the &amp; as being removed and replaced with the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF2E2F3E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*compiled*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2E2F3E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  parent selector. </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1932,6 +2240,33 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFDC143C"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2E2F3E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF2E2F3E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1975,7 +2310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2100,6 +2435,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2122,6 +2464,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2523,8 +2871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2721,10 +3069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D114"/>
+  <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="B105" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2789,7 +3137,7 @@
       <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="47" t="s">
+      <c r="D9" s="50" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2798,37 +3146,37 @@
       <c r="C10" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="D10" s="47"/>
+      <c r="D10" s="50"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="50"/>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="D12" s="47"/>
+      <c r="D12" s="50"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="47"/>
+      <c r="D13" s="50"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="47"/>
+      <c r="D14" s="50"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="47"/>
+      <c r="D15" s="50"/>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
@@ -2856,7 +3204,7 @@
       <c r="C20" t="s">
         <v>168</v>
       </c>
-      <c r="D20" s="51" t="s">
+      <c r="D20" s="54" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2864,25 +3212,25 @@
       <c r="C21" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="D21" s="51"/>
+      <c r="D21" s="54"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="51"/>
+      <c r="D22" s="54"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="51"/>
+      <c r="D23" s="54"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="51"/>
+      <c r="D24" s="54"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
@@ -2979,7 +3327,7 @@
       <c r="C41" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="49" t="s">
+      <c r="D41" s="52" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2987,31 +3335,31 @@
       <c r="C42" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="49"/>
+      <c r="D42" s="52"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>67</v>
       </c>
-      <c r="D43" s="49"/>
+      <c r="D43" s="52"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="49"/>
+      <c r="D44" s="52"/>
     </row>
     <row r="45" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C45" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="49"/>
+      <c r="D45" s="52"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>70</v>
       </c>
-      <c r="D46" s="49"/>
+      <c r="D46" s="52"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
@@ -3025,7 +3373,7 @@
       <c r="C49" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D49" s="50" t="s">
+      <c r="D49" s="53" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3033,7 +3381,7 @@
       <c r="C50" t="s">
         <v>74</v>
       </c>
-      <c r="D50" s="50"/>
+      <c r="D50" s="53"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
@@ -3206,7 +3554,7 @@
       <c r="C82" t="s">
         <v>106</v>
       </c>
-      <c r="D82" s="48" t="s">
+      <c r="D82" s="51" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3214,31 +3562,31 @@
       <c r="C83" t="s">
         <v>107</v>
       </c>
-      <c r="D83" s="48"/>
+      <c r="D83" s="51"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>108</v>
       </c>
-      <c r="D84" s="48"/>
+      <c r="D84" s="51"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
         <v>109</v>
       </c>
-      <c r="D85" s="48"/>
+      <c r="D85" s="51"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
         <v>111</v>
       </c>
-      <c r="D86" s="48"/>
+      <c r="D86" s="51"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
         <v>112</v>
       </c>
-      <c r="D87" s="48"/>
+      <c r="D87" s="51"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
@@ -3328,7 +3676,7 @@
       <c r="C106" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="D106" s="48" t="s">
+      <c r="D106" s="51" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3336,28 +3684,28 @@
       <c r="C107" t="s">
         <v>211</v>
       </c>
-      <c r="D107" s="48"/>
+      <c r="D107" s="51"/>
     </row>
     <row r="108" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C108" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="D108" s="48"/>
+      <c r="D108" s="51"/>
     </row>
     <row r="109" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C109" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="D109" s="48"/>
+      <c r="D109" s="51"/>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C110" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="D110" s="48"/>
+      <c r="D110" s="51"/>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D111" s="48"/>
+      <c r="D111" s="51"/>
     </row>
     <row r="112" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C112" t="s">
@@ -3367,14 +3715,22 @@
         <v>252</v>
       </c>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C113" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C114" s="12" t="s">
         <v>250</v>
+      </c>
+    </row>
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>287</v>
+      </c>
+      <c r="D116" s="12" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -3404,9 +3760,10 @@
     <hyperlink ref="C70" r:id="rId3" location="the-data-flows-down" display="https://reactjs.org/docs/state-and-lifecycle.html - the-data-flows-down"/>
     <hyperlink ref="C110" r:id="rId4" display="match.url helps us make a relative path https://stackoverflow.com/questions/46096518/what-exactly-is-dynamic-routing-in-reactjs"/>
     <hyperlink ref="C114" r:id="rId5"/>
+    <hyperlink ref="D116" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -3415,7 +3772,7 @@
   <dimension ref="C4:G75"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3593,13 +3950,13 @@
       <c r="F23" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="G23" s="52" t="s">
+      <c r="G23" s="55" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D24" s="22"/>
-      <c r="G24" s="52"/>
+      <c r="G24" s="55"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D25" s="17" t="s">
@@ -3608,34 +3965,34 @@
       <c r="E25" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="G25" s="52"/>
+      <c r="G25" s="55"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="G26" s="52"/>
+      <c r="G26" s="55"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="52"/>
+      <c r="G27" s="55"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="G28" s="52"/>
+      <c r="G28" s="55"/>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="G29" s="52"/>
+      <c r="G29" s="55"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D30" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="G30" s="52"/>
+      <c r="G30" s="55"/>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="G31" s="52"/>
+      <c r="G31" s="55"/>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="G32" s="52"/>
+      <c r="G32" s="55"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="52"/>
+      <c r="G33" s="55"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D34" s="17" t="s">
@@ -3644,7 +4001,7 @@
       <c r="E34" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="G34" s="52"/>
+      <c r="G34" s="55"/>
     </row>
     <row r="35" spans="3:7" ht="45" x14ac:dyDescent="0.25">
       <c r="E35" s="37" t="s">
@@ -3729,42 +4086,42 @@
       <c r="D62" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="E62" s="53" t="s">
+      <c r="E62" s="56" t="s">
         <v>226</v>
       </c>
-      <c r="F62" s="53"/>
+      <c r="F62" s="56"/>
       <c r="G62" s="35" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E63" s="53" t="s">
+      <c r="E63" s="56" t="s">
         <v>227</v>
       </c>
-      <c r="F63" s="53"/>
+      <c r="F63" s="56"/>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E64" s="53" t="s">
+      <c r="E64" s="56" t="s">
         <v>228</v>
       </c>
-      <c r="F64" s="53"/>
-      <c r="G64" s="54" t="s">
+      <c r="F64" s="56"/>
+      <c r="G64" s="57" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E65" s="53" t="s">
+      <c r="E65" s="56" t="s">
         <v>229</v>
       </c>
-      <c r="F65" s="53"/>
-      <c r="G65" s="54"/>
+      <c r="F65" s="56"/>
+      <c r="G65" s="57"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E66" s="53" t="s">
+      <c r="E66" s="56" t="s">
         <v>230</v>
       </c>
-      <c r="F66" s="53"/>
-      <c r="G66" s="54"/>
+      <c r="F66" s="56"/>
+      <c r="G66" s="57"/>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C68" s="20" t="s">
@@ -3852,73 +4209,354 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:D19"/>
+  <dimension ref="B3:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="48"/>
+    <col min="2" max="2" width="13.28515625" style="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" style="48" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="48" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" style="48" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="48"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>289</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="48" t="s">
+        <v>291</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5" s="46" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C6" s="46" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C7" s="46" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>270</v>
-      </c>
-      <c r="D19" t="s">
-        <v>271</v>
+    <row r="9" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="48" t="s">
+        <v>321</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>322</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="C22" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:G18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="D5" t="s">
+        <v>313</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>266</v>
+      </c>
+      <c r="E7" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>269</v>
+      </c>
+      <c r="E11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="D12" s="58" t="s">
+        <v>317</v>
+      </c>
+      <c r="G12" s="47" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E13" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="3:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="19" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="D17" s="48" t="s">
+        <v>315</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>319</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:F20"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.28515625" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.140625" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>272</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="D5" t="s">
+        <v>283</v>
+      </c>
+      <c r="E5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="D6" t="s">
+        <v>271</v>
+      </c>
+      <c r="E6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="48" t="s">
+        <v>295</v>
+      </c>
+      <c r="D7" t="s">
+        <v>277</v>
+      </c>
+      <c r="E7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="48" t="s">
+        <v>296</v>
+      </c>
+      <c r="D8" t="s">
+        <v>279</v>
+      </c>
+      <c r="E8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>281</v>
+      </c>
+      <c r="E9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="20" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="C13" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D16" s="47" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="C18" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="D20" s="47" t="s">
+        <v>306</v>
+      </c>
+      <c r="E20" s="47" t="s">
+        <v>307</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="diff bet HTML and HTML5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>